<commit_message>
Ajuste dos pesos e adicionando lipideos
</commit_message>
<xml_diff>
--- a/carolina_dados.xlsx
+++ b/carolina_dados.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N295"/>
+  <dimension ref="A1:O295"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -504,6 +504,11 @@
           <t>Pesos</t>
         </is>
       </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Lipídeos</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -552,6 +557,9 @@
       <c r="N2" t="n">
         <v>0</v>
       </c>
+      <c r="O2" t="n">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -598,6 +606,9 @@
         </is>
       </c>
       <c r="N3" t="n">
+        <v>1</v>
+      </c>
+      <c r="O3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -646,7 +657,10 @@
         </is>
       </c>
       <c r="N4" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0.1</v>
       </c>
     </row>
     <row r="5">
@@ -696,6 +710,9 @@
       <c r="N5" t="n">
         <v>1</v>
       </c>
+      <c r="O5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -744,6 +761,9 @@
       <c r="N6" t="n">
         <v>0</v>
       </c>
+      <c r="O6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -790,7 +810,10 @@
         </is>
       </c>
       <c r="N7" t="n">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -840,6 +863,9 @@
       <c r="N8" t="n">
         <v>0</v>
       </c>
+      <c r="O8" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -888,6 +914,9 @@
       <c r="N9" t="n">
         <v>0</v>
       </c>
+      <c r="O9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -936,6 +965,9 @@
       <c r="N10" t="n">
         <v>0</v>
       </c>
+      <c r="O10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -984,6 +1016,9 @@
       <c r="N11" t="n">
         <v>0</v>
       </c>
+      <c r="O11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1032,6 +1067,9 @@
       <c r="N12" t="n">
         <v>0</v>
       </c>
+      <c r="O12" t="n">
+        <v>1.9</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1080,6 +1118,9 @@
       <c r="N13" t="n">
         <v>0</v>
       </c>
+      <c r="O13" t="n">
+        <v>3.6</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1128,6 +1169,9 @@
       <c r="N14" t="n">
         <v>0</v>
       </c>
+      <c r="O14" t="n">
+        <v>2.2</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1176,6 +1220,9 @@
       <c r="N15" t="n">
         <v>0</v>
       </c>
+      <c r="O15" t="n">
+        <v>0.9</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1224,6 +1271,9 @@
       <c r="N16" t="n">
         <v>0</v>
       </c>
+      <c r="O16" t="n">
+        <v>26.9</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1272,6 +1322,9 @@
       <c r="N17" t="n">
         <v>0</v>
       </c>
+      <c r="O17" t="n">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1320,6 +1373,9 @@
       <c r="N18" t="n">
         <v>0</v>
       </c>
+      <c r="O18" t="n">
+        <v>1.9</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1368,6 +1424,9 @@
       <c r="N19" t="n">
         <v>0</v>
       </c>
+      <c r="O19" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1416,6 +1475,9 @@
       <c r="N20" t="n">
         <v>0</v>
       </c>
+      <c r="O20" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1464,6 +1526,9 @@
       <c r="N21" t="n">
         <v>0</v>
       </c>
+      <c r="O21" t="n">
+        <v>2.3</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1512,6 +1577,9 @@
       <c r="N22" t="n">
         <v>0</v>
       </c>
+      <c r="O22" t="n">
+        <v>2.3</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1560,6 +1628,9 @@
       <c r="N23" t="n">
         <v>0</v>
       </c>
+      <c r="O23" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1608,6 +1679,9 @@
       <c r="N24" t="n">
         <v>0</v>
       </c>
+      <c r="O24" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1656,6 +1730,9 @@
       <c r="N25" t="n">
         <v>0</v>
       </c>
+      <c r="O25" t="n">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1702,7 +1779,10 @@
         </is>
       </c>
       <c r="N26" t="n">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="O26" t="n">
+        <v>0.1</v>
       </c>
     </row>
     <row r="27">
@@ -1752,6 +1832,9 @@
       <c r="N27" t="n">
         <v>0</v>
       </c>
+      <c r="O27" t="n">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1800,6 +1883,9 @@
       <c r="N28" t="n">
         <v>0</v>
       </c>
+      <c r="O28" t="n">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1848,6 +1934,9 @@
       <c r="N29" t="n">
         <v>0</v>
       </c>
+      <c r="O29" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1894,7 +1983,10 @@
         </is>
       </c>
       <c r="N30" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="O30" t="n">
+        <v>0.1</v>
       </c>
     </row>
     <row r="31">
@@ -1944,6 +2036,9 @@
       <c r="N31" t="n">
         <v>0</v>
       </c>
+      <c r="O31" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1992,6 +2087,9 @@
       <c r="N32" t="n">
         <v>0</v>
       </c>
+      <c r="O32" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -2040,6 +2138,9 @@
       <c r="N33" t="n">
         <v>0</v>
       </c>
+      <c r="O33" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -2088,6 +2189,9 @@
       <c r="N34" t="n">
         <v>0</v>
       </c>
+      <c r="O34" t="n">
+        <v>8.4</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -2136,6 +2240,9 @@
       <c r="N35" t="n">
         <v>0</v>
       </c>
+      <c r="O35" t="n">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -2184,6 +2291,9 @@
       <c r="N36" t="n">
         <v>0</v>
       </c>
+      <c r="O36" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -2232,6 +2342,9 @@
       <c r="N37" t="n">
         <v>0</v>
       </c>
+      <c r="O37" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -2280,6 +2393,9 @@
       <c r="N38" t="n">
         <v>0</v>
       </c>
+      <c r="O38" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -2328,6 +2444,9 @@
       <c r="N39" t="n">
         <v>0</v>
       </c>
+      <c r="O39" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -2376,6 +2495,9 @@
       <c r="N40" t="n">
         <v>0</v>
       </c>
+      <c r="O40" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -2424,6 +2546,9 @@
       <c r="N41" t="n">
         <v>0</v>
       </c>
+      <c r="O41" t="n">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -2472,6 +2597,9 @@
       <c r="N42" t="n">
         <v>0</v>
       </c>
+      <c r="O42" t="n">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -2518,7 +2646,10 @@
         </is>
       </c>
       <c r="N43" t="n">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="O43" t="n">
+        <v>0.1</v>
       </c>
     </row>
     <row r="44">
@@ -2568,6 +2699,9 @@
       <c r="N44" t="n">
         <v>0</v>
       </c>
+      <c r="O44" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -2616,6 +2750,9 @@
       <c r="N45" t="n">
         <v>0</v>
       </c>
+      <c r="O45" t="n">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -2664,6 +2801,9 @@
       <c r="N46" t="n">
         <v>0</v>
       </c>
+      <c r="O46" t="n">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -2712,6 +2852,9 @@
       <c r="N47" t="n">
         <v>0</v>
       </c>
+      <c r="O47" t="n">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -2760,6 +2903,9 @@
       <c r="N48" t="n">
         <v>0</v>
       </c>
+      <c r="O48" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -2808,6 +2954,9 @@
       <c r="N49" t="n">
         <v>0</v>
       </c>
+      <c r="O49" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -2856,6 +3005,9 @@
       <c r="N50" t="n">
         <v>0</v>
       </c>
+      <c r="O50" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -2904,6 +3056,9 @@
       <c r="N51" t="n">
         <v>0</v>
       </c>
+      <c r="O51" t="n">
+        <v>0.4</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -2952,6 +3107,9 @@
       <c r="N52" t="n">
         <v>0</v>
       </c>
+      <c r="O52" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -3000,6 +3158,9 @@
       <c r="N53" t="n">
         <v>0</v>
       </c>
+      <c r="O53" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -3048,6 +3209,9 @@
       <c r="N54" t="n">
         <v>0</v>
       </c>
+      <c r="O54" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -3096,6 +3260,9 @@
       <c r="N55" t="n">
         <v>0</v>
       </c>
+      <c r="O55" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -3144,6 +3311,9 @@
       <c r="N56" t="n">
         <v>0</v>
       </c>
+      <c r="O56" t="n">
+        <v>0.4</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -3192,6 +3362,9 @@
       <c r="N57" t="n">
         <v>0</v>
       </c>
+      <c r="O57" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -3240,6 +3413,9 @@
       <c r="N58" t="n">
         <v>0</v>
       </c>
+      <c r="O58" t="n">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -3288,6 +3464,9 @@
       <c r="N59" t="n">
         <v>0</v>
       </c>
+      <c r="O59" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -3336,6 +3515,9 @@
       <c r="N60" t="n">
         <v>0</v>
       </c>
+      <c r="O60" t="n">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -3384,6 +3566,9 @@
       <c r="N61" t="n">
         <v>0</v>
       </c>
+      <c r="O61" t="n">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -3432,6 +3617,9 @@
       <c r="N62" t="n">
         <v>0</v>
       </c>
+      <c r="O62" t="n">
+        <v>0.6</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -3480,6 +3668,9 @@
       <c r="N63" t="n">
         <v>0</v>
       </c>
+      <c r="O63" t="n">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -3528,6 +3719,9 @@
       <c r="N64" t="n">
         <v>0</v>
       </c>
+      <c r="O64" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -3576,6 +3770,9 @@
       <c r="N65" t="n">
         <v>0</v>
       </c>
+      <c r="O65" t="n">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -3624,6 +3821,9 @@
       <c r="N66" t="n">
         <v>0</v>
       </c>
+      <c r="O66" t="n">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -3672,6 +3872,9 @@
       <c r="N67" t="n">
         <v>0</v>
       </c>
+      <c r="O67" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -3720,6 +3923,9 @@
       <c r="N68" t="n">
         <v>0</v>
       </c>
+      <c r="O68" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -3768,6 +3974,9 @@
       <c r="N69" t="n">
         <v>0</v>
       </c>
+      <c r="O69" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -3816,6 +4025,9 @@
       <c r="N70" t="n">
         <v>0</v>
       </c>
+      <c r="O70" t="n">
+        <v>40.7</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -3864,6 +4076,9 @@
       <c r="N71" t="n">
         <v>0</v>
       </c>
+      <c r="O71" t="n">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -3910,7 +4125,10 @@
         </is>
       </c>
       <c r="N72" t="n">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="O72" t="n">
+        <v>0.1</v>
       </c>
     </row>
     <row r="73">
@@ -3960,6 +4178,9 @@
       <c r="N73" t="n">
         <v>0</v>
       </c>
+      <c r="O73" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -4008,6 +4229,9 @@
       <c r="N74" t="n">
         <v>0</v>
       </c>
+      <c r="O74" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -4056,6 +4280,9 @@
       <c r="N75" t="n">
         <v>0</v>
       </c>
+      <c r="O75" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -4104,6 +4331,9 @@
       <c r="N76" t="n">
         <v>0</v>
       </c>
+      <c r="O76" t="n">
+        <v>2.1</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -4152,6 +4382,9 @@
       <c r="N77" t="n">
         <v>0</v>
       </c>
+      <c r="O77" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -4200,6 +4433,9 @@
       <c r="N78" t="n">
         <v>0</v>
       </c>
+      <c r="O78" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -4248,6 +4484,9 @@
       <c r="N79" t="n">
         <v>0</v>
       </c>
+      <c r="O79" t="n">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -4296,6 +4535,9 @@
       <c r="N80" t="n">
         <v>0</v>
       </c>
+      <c r="O80" t="n">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -4342,7 +4584,10 @@
         </is>
       </c>
       <c r="N81" t="n">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="O81" t="n">
+        <v>0.3</v>
       </c>
     </row>
     <row r="82">
@@ -4392,6 +4637,9 @@
       <c r="N82" t="n">
         <v>0</v>
       </c>
+      <c r="O82" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -4440,6 +4688,9 @@
       <c r="N83" t="n">
         <v>0</v>
       </c>
+      <c r="O83" t="n">
+        <v>18</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -4488,6 +4739,9 @@
       <c r="N84" t="n">
         <v>0</v>
       </c>
+      <c r="O84" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -4536,6 +4790,9 @@
       <c r="N85" t="n">
         <v>0</v>
       </c>
+      <c r="O85" t="n">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -4584,6 +4841,9 @@
       <c r="N86" t="n">
         <v>0</v>
       </c>
+      <c r="O86" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -4632,6 +4892,9 @@
       <c r="N87" t="n">
         <v>0</v>
       </c>
+      <c r="O87" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -4680,6 +4943,9 @@
       <c r="N88" t="n">
         <v>0</v>
       </c>
+      <c r="O88" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -4728,6 +4994,9 @@
       <c r="N89" t="n">
         <v>0</v>
       </c>
+      <c r="O89" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -4776,6 +5045,9 @@
       <c r="N90" t="n">
         <v>0</v>
       </c>
+      <c r="O90" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -4824,6 +5096,9 @@
       <c r="N91" t="n">
         <v>0</v>
       </c>
+      <c r="O91" t="n">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -4870,7 +5145,10 @@
         </is>
       </c>
       <c r="N92" t="n">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="O92" t="n">
+        <v>19.1</v>
       </c>
     </row>
     <row r="93">
@@ -4920,6 +5198,9 @@
       <c r="N93" t="n">
         <v>0</v>
       </c>
+      <c r="O93" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -4968,6 +5249,9 @@
       <c r="N94" t="n">
         <v>0</v>
       </c>
+      <c r="O94" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -5016,6 +5300,9 @@
       <c r="N95" t="n">
         <v>0</v>
       </c>
+      <c r="O95" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -5064,6 +5351,9 @@
       <c r="N96" t="n">
         <v>0</v>
       </c>
+      <c r="O96" t="n">
+        <v>1.9</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -5112,6 +5402,9 @@
       <c r="N97" t="n">
         <v>0</v>
       </c>
+      <c r="O97" t="n">
+        <v>3.04</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -5160,6 +5453,9 @@
       <c r="N98" t="n">
         <v>0</v>
       </c>
+      <c r="O98" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -5208,6 +5504,9 @@
       <c r="N99" t="n">
         <v>0</v>
       </c>
+      <c r="O99" t="n">
+        <v>2.3</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -5256,6 +5555,9 @@
       <c r="N100" t="n">
         <v>0</v>
       </c>
+      <c r="O100" t="n">
+        <v>2.3</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -5304,6 +5606,9 @@
       <c r="N101" t="n">
         <v>0</v>
       </c>
+      <c r="O101" t="n">
+        <v>3.8</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -5352,6 +5657,9 @@
       <c r="N102" t="n">
         <v>0</v>
       </c>
+      <c r="O102" t="n">
+        <v>2.2</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -5400,6 +5708,9 @@
       <c r="N103" t="n">
         <v>0</v>
       </c>
+      <c r="O103" t="n">
+        <v>0.9</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -5448,6 +5759,9 @@
       <c r="N104" t="n">
         <v>0</v>
       </c>
+      <c r="O104" t="n">
+        <v>26.9</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -5496,6 +5810,9 @@
       <c r="N105" t="n">
         <v>0</v>
       </c>
+      <c r="O105" t="n">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -5544,6 +5861,9 @@
       <c r="N106" t="n">
         <v>0</v>
       </c>
+      <c r="O106" t="n">
+        <v>20.2</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -5592,6 +5912,9 @@
       <c r="N107" t="n">
         <v>0</v>
       </c>
+      <c r="O107" t="n">
+        <v>24.6</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -5640,6 +5963,9 @@
       <c r="N108" t="n">
         <v>0</v>
       </c>
+      <c r="O108" t="n">
+        <v>25.2</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -5688,6 +6014,9 @@
       <c r="N109" t="n">
         <v>0</v>
       </c>
+      <c r="O109" t="n">
+        <v>33.5</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -5736,6 +6065,9 @@
       <c r="N110" t="n">
         <v>0</v>
       </c>
+      <c r="O110" t="n">
+        <v>27.4</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -5784,6 +6116,9 @@
       <c r="N111" t="n">
         <v>0</v>
       </c>
+      <c r="O111" t="n">
+        <v>2.8</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -5832,6 +6167,9 @@
       <c r="N112" t="n">
         <v>0</v>
       </c>
+      <c r="O112" t="n">
+        <v>29.1</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -5880,6 +6218,9 @@
       <c r="N113" t="n">
         <v>0</v>
       </c>
+      <c r="O113" t="n">
+        <v>23.4</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -5926,7 +6267,10 @@
         </is>
       </c>
       <c r="N114" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="O114" t="n">
+        <v>8.1</v>
       </c>
     </row>
     <row r="115">
@@ -5976,6 +6320,9 @@
       <c r="N115" t="n">
         <v>0</v>
       </c>
+      <c r="O115" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -6024,6 +6371,9 @@
       <c r="N116" t="n">
         <v>0</v>
       </c>
+      <c r="O116" t="n">
+        <v>19.6</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -6072,6 +6422,9 @@
       <c r="N117" t="n">
         <v>0</v>
       </c>
+      <c r="O117" t="n">
+        <v>19.6</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -6120,6 +6473,9 @@
       <c r="N118" t="n">
         <v>0</v>
       </c>
+      <c r="O118" t="n">
+        <v>24.7</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -6168,6 +6524,9 @@
       <c r="N119" t="n">
         <v>0</v>
       </c>
+      <c r="O119" t="n">
+        <v>26.4</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -6216,6 +6575,9 @@
       <c r="N120" t="n">
         <v>0</v>
       </c>
+      <c r="O120" t="n">
+        <v>14.4</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -6264,6 +6626,9 @@
       <c r="N121" t="n">
         <v>0</v>
       </c>
+      <c r="O121" t="n">
+        <v>12.7</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -6312,6 +6677,9 @@
       <c r="N122" t="n">
         <v>0</v>
       </c>
+      <c r="O122" t="n">
+        <v>18.5</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -6360,6 +6728,9 @@
       <c r="N123" t="n">
         <v>0</v>
       </c>
+      <c r="O123" t="n">
+        <v>11.3</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -6408,6 +6779,9 @@
       <c r="N124" t="n">
         <v>0</v>
       </c>
+      <c r="O124" t="n">
+        <v>12.4</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -6456,6 +6830,9 @@
       <c r="N125" t="n">
         <v>0</v>
       </c>
+      <c r="O125" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -6504,6 +6881,9 @@
       <c r="N126" t="n">
         <v>0</v>
       </c>
+      <c r="O126" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -6550,7 +6930,10 @@
         </is>
       </c>
       <c r="N127" t="n">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="O127" t="n">
+        <v>1.6</v>
       </c>
     </row>
     <row r="128">
@@ -6600,6 +6983,9 @@
       <c r="N128" t="n">
         <v>0</v>
       </c>
+      <c r="O128" t="n">
+        <v>5.7</v>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -6648,6 +7034,9 @@
       <c r="N129" t="n">
         <v>0</v>
       </c>
+      <c r="O129" t="n">
+        <v>3.6</v>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -6694,7 +7083,10 @@
         </is>
       </c>
       <c r="N130" t="n">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="O130" t="n">
+        <v>2.7</v>
       </c>
     </row>
     <row r="131">
@@ -6744,6 +7136,9 @@
       <c r="N131" t="n">
         <v>0</v>
       </c>
+      <c r="O131" t="n">
+        <v>3.1</v>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -6790,7 +7185,10 @@
         </is>
       </c>
       <c r="N132" t="n">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="O132" t="n">
+        <v>3.7</v>
       </c>
     </row>
     <row r="133">
@@ -6840,6 +7238,9 @@
       <c r="N133" t="n">
         <v>0</v>
       </c>
+      <c r="O133" t="n">
+        <v>3.1</v>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -6888,6 +7289,9 @@
       <c r="N134" t="n">
         <v>0</v>
       </c>
+      <c r="O134" t="n">
+        <v>2.8</v>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -6936,6 +7340,9 @@
       <c r="N135" t="n">
         <v>0</v>
       </c>
+      <c r="O135" t="n">
+        <v>24.6</v>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -6984,6 +7391,9 @@
       <c r="N136" t="n">
         <v>0</v>
       </c>
+      <c r="O136" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -7032,6 +7442,9 @@
       <c r="N137" t="n">
         <v>0</v>
       </c>
+      <c r="O137" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -7080,6 +7493,9 @@
       <c r="N138" t="n">
         <v>0</v>
       </c>
+      <c r="O138" t="n">
+        <v>0.4</v>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -7128,6 +7544,9 @@
       <c r="N139" t="n">
         <v>0</v>
       </c>
+      <c r="O139" t="n">
+        <v>1.2</v>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -7176,6 +7595,9 @@
       <c r="N140" t="n">
         <v>0</v>
       </c>
+      <c r="O140" t="n">
+        <v>17.2</v>
+      </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -7224,6 +7646,9 @@
       <c r="N141" t="n">
         <v>0</v>
       </c>
+      <c r="O141" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -7272,6 +7697,9 @@
       <c r="N142" t="n">
         <v>0</v>
       </c>
+      <c r="O142" t="n">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -7318,7 +7746,10 @@
         </is>
       </c>
       <c r="N143" t="n">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="O143" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="144">
@@ -7368,6 +7799,9 @@
       <c r="N144" t="n">
         <v>0</v>
       </c>
+      <c r="O144" t="n">
+        <v>13.1</v>
+      </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -7414,7 +7848,10 @@
         </is>
       </c>
       <c r="N145" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="O145" t="n">
+        <v>0.9</v>
       </c>
     </row>
     <row r="146">
@@ -7464,6 +7901,9 @@
       <c r="N146" t="n">
         <v>0</v>
       </c>
+      <c r="O146" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -7512,6 +7952,9 @@
       <c r="N147" t="n">
         <v>0</v>
       </c>
+      <c r="O147" t="n">
+        <v>11.2</v>
+      </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -7560,6 +8003,9 @@
       <c r="N148" t="n">
         <v>0</v>
       </c>
+      <c r="O148" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -7608,6 +8054,9 @@
       <c r="N149" t="n">
         <v>0</v>
       </c>
+      <c r="O149" t="n">
+        <v>0.4</v>
+      </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
@@ -7656,6 +8105,9 @@
       <c r="N150" t="n">
         <v>0</v>
       </c>
+      <c r="O150" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
@@ -7704,6 +8156,9 @@
       <c r="N151" t="n">
         <v>0</v>
       </c>
+      <c r="O151" t="n">
+        <v>0.6</v>
+      </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
@@ -7752,6 +8207,9 @@
       <c r="N152" t="n">
         <v>0</v>
       </c>
+      <c r="O152" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
@@ -7800,6 +8258,9 @@
       <c r="N153" t="n">
         <v>0</v>
       </c>
+      <c r="O153" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
@@ -7848,6 +8309,9 @@
       <c r="N154" t="n">
         <v>0</v>
       </c>
+      <c r="O154" t="n">
+        <v>0.4</v>
+      </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -7894,7 +8358,10 @@
         </is>
       </c>
       <c r="N155" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="O155" t="n">
+        <v>0.5</v>
       </c>
     </row>
     <row r="156">
@@ -7944,6 +8411,9 @@
       <c r="N156" t="n">
         <v>0</v>
       </c>
+      <c r="O156" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
@@ -7990,7 +8460,10 @@
         </is>
       </c>
       <c r="N157" t="n">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="O157" t="n">
+        <v>0.5</v>
       </c>
     </row>
     <row r="158">
@@ -8038,7 +8511,10 @@
         </is>
       </c>
       <c r="N158" t="n">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="O158" t="n">
+        <v>1.6</v>
       </c>
     </row>
     <row r="159">
@@ -8086,7 +8562,10 @@
         </is>
       </c>
       <c r="N159" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="O159" t="n">
+        <v>26.2</v>
       </c>
     </row>
     <row r="160">
@@ -8134,7 +8613,10 @@
         </is>
       </c>
       <c r="N160" t="n">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="O160" t="n">
+        <v>0.7</v>
       </c>
     </row>
     <row r="161">
@@ -8184,6 +8666,9 @@
       <c r="N161" t="n">
         <v>0</v>
       </c>
+      <c r="O161" t="n">
+        <v>0.8</v>
+      </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
@@ -8232,6 +8717,9 @@
       <c r="N162" t="n">
         <v>0</v>
       </c>
+      <c r="O162" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
@@ -8280,6 +8768,9 @@
       <c r="N163" t="n">
         <v>0</v>
       </c>
+      <c r="O163" t="n">
+        <v>0.8</v>
+      </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
@@ -8328,6 +8819,9 @@
       <c r="N164" t="n">
         <v>0</v>
       </c>
+      <c r="O164" t="n">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
@@ -8376,6 +8870,9 @@
       <c r="N165" t="n">
         <v>0</v>
       </c>
+      <c r="O165" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
@@ -8424,6 +8921,9 @@
       <c r="N166" t="n">
         <v>0</v>
       </c>
+      <c r="O166" t="n">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
@@ -8472,6 +8972,9 @@
       <c r="N167" t="n">
         <v>0</v>
       </c>
+      <c r="O167" t="n">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
@@ -8520,6 +9023,9 @@
       <c r="N168" t="n">
         <v>0</v>
       </c>
+      <c r="O168" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
@@ -8568,6 +9074,9 @@
       <c r="N169" t="n">
         <v>0</v>
       </c>
+      <c r="O169" t="n">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
@@ -8616,6 +9125,9 @@
       <c r="N170" t="n">
         <v>0</v>
       </c>
+      <c r="O170" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
@@ -8664,6 +9176,9 @@
       <c r="N171" t="n">
         <v>0</v>
       </c>
+      <c r="O171" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
@@ -8712,6 +9227,9 @@
       <c r="N172" t="n">
         <v>0</v>
       </c>
+      <c r="O172" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
@@ -8760,6 +9278,9 @@
       <c r="N173" t="n">
         <v>0</v>
       </c>
+      <c r="O173" t="n">
+        <v>4.8</v>
+      </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
@@ -8808,6 +9329,9 @@
       <c r="N174" t="n">
         <v>0</v>
       </c>
+      <c r="O174" t="n">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
@@ -8856,6 +9380,9 @@
       <c r="N175" t="n">
         <v>0</v>
       </c>
+      <c r="O175" t="n">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
@@ -8904,6 +9431,9 @@
       <c r="N176" t="n">
         <v>0</v>
       </c>
+      <c r="O176" t="n">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
@@ -8952,6 +9482,9 @@
       <c r="N177" t="n">
         <v>0</v>
       </c>
+      <c r="O177" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
@@ -9000,6 +9533,9 @@
       <c r="N178" t="n">
         <v>0</v>
       </c>
+      <c r="O178" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
@@ -9048,6 +9584,9 @@
       <c r="N179" t="n">
         <v>0</v>
       </c>
+      <c r="O179" t="n">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
@@ -9096,6 +9635,9 @@
       <c r="N180" t="n">
         <v>0</v>
       </c>
+      <c r="O180" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
@@ -9144,6 +9686,9 @@
       <c r="N181" t="n">
         <v>0</v>
       </c>
+      <c r="O181" t="n">
+        <v>4.8</v>
+      </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
@@ -9192,6 +9737,9 @@
       <c r="N182" t="n">
         <v>0</v>
       </c>
+      <c r="O182" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
@@ -9240,6 +9788,9 @@
       <c r="N183" t="n">
         <v>0</v>
       </c>
+      <c r="O183" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
@@ -9288,6 +9839,9 @@
       <c r="N184" t="n">
         <v>0</v>
       </c>
+      <c r="O184" t="n">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
@@ -9336,6 +9890,9 @@
       <c r="N185" t="n">
         <v>0</v>
       </c>
+      <c r="O185" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
@@ -9384,6 +9941,9 @@
       <c r="N186" t="n">
         <v>0</v>
       </c>
+      <c r="O186" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
@@ -9432,6 +9992,9 @@
       <c r="N187" t="n">
         <v>0</v>
       </c>
+      <c r="O187" t="n">
+        <v>6.6</v>
+      </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
@@ -9480,6 +10043,9 @@
       <c r="N188" t="n">
         <v>0</v>
       </c>
+      <c r="O188" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
@@ -9528,6 +10094,9 @@
       <c r="N189" t="n">
         <v>0</v>
       </c>
+      <c r="O189" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
@@ -9576,6 +10145,9 @@
       <c r="N190" t="n">
         <v>0</v>
       </c>
+      <c r="O190" t="n">
+        <v>5.4</v>
+      </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
@@ -9624,6 +10196,9 @@
       <c r="N191" t="n">
         <v>0</v>
       </c>
+      <c r="O191" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
@@ -9670,7 +10245,10 @@
         </is>
       </c>
       <c r="N192" t="n">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="O192" t="n">
+        <v>0.4</v>
       </c>
     </row>
     <row r="193">
@@ -9720,6 +10298,9 @@
       <c r="N193" t="n">
         <v>0</v>
       </c>
+      <c r="O193" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
@@ -9766,6 +10347,9 @@
         </is>
       </c>
       <c r="N194" t="n">
+        <v>1</v>
+      </c>
+      <c r="O194" t="n">
         <v>0</v>
       </c>
     </row>
@@ -9816,6 +10400,9 @@
       <c r="N195" t="n">
         <v>0</v>
       </c>
+      <c r="O195" t="n">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
@@ -9864,6 +10451,9 @@
       <c r="N196" t="n">
         <v>0</v>
       </c>
+      <c r="O196" t="n">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
@@ -9912,6 +10502,9 @@
       <c r="N197" t="n">
         <v>0</v>
       </c>
+      <c r="O197" t="n">
+        <v>1.2</v>
+      </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
@@ -9958,7 +10551,10 @@
         </is>
       </c>
       <c r="N198" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="O198" t="n">
+        <v>0.1</v>
       </c>
     </row>
     <row r="199">
@@ -10008,6 +10604,9 @@
       <c r="N199" t="n">
         <v>0</v>
       </c>
+      <c r="O199" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
@@ -10056,6 +10655,9 @@
       <c r="N200" t="n">
         <v>0</v>
       </c>
+      <c r="O200" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
@@ -10104,6 +10706,9 @@
       <c r="N201" t="n">
         <v>0</v>
       </c>
+      <c r="O201" t="n">
+        <v>1.2</v>
+      </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
@@ -10152,6 +10757,9 @@
       <c r="N202" t="n">
         <v>0</v>
       </c>
+      <c r="O202" t="n">
+        <v>0.9</v>
+      </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
@@ -10200,6 +10808,9 @@
       <c r="N203" t="n">
         <v>0</v>
       </c>
+      <c r="O203" t="n">
+        <v>1.3</v>
+      </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
@@ -10248,6 +10859,9 @@
       <c r="N204" t="n">
         <v>0</v>
       </c>
+      <c r="O204" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
@@ -10296,6 +10910,9 @@
       <c r="N205" t="n">
         <v>0</v>
       </c>
+      <c r="O205" t="n">
+        <v>3.6</v>
+      </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
@@ -10344,6 +10961,9 @@
       <c r="N206" t="n">
         <v>0</v>
       </c>
+      <c r="O206" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
@@ -10392,6 +11012,9 @@
       <c r="N207" t="n">
         <v>0</v>
       </c>
+      <c r="O207" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
@@ -10440,6 +11063,9 @@
       <c r="N208" t="n">
         <v>0</v>
       </c>
+      <c r="O208" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
@@ -10488,6 +11114,9 @@
       <c r="N209" t="n">
         <v>0</v>
       </c>
+      <c r="O209" t="n">
+        <v>15.6</v>
+      </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
@@ -10536,6 +11165,9 @@
       <c r="N210" t="n">
         <v>0</v>
       </c>
+      <c r="O210" t="n">
+        <v>0.4</v>
+      </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
@@ -10584,6 +11216,9 @@
       <c r="N211" t="n">
         <v>0</v>
       </c>
+      <c r="O211" t="n">
+        <v>19.6</v>
+      </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
@@ -10632,6 +11267,9 @@
       <c r="N212" t="n">
         <v>0</v>
       </c>
+      <c r="O212" t="n">
+        <v>16.9</v>
+      </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
@@ -10680,6 +11318,9 @@
       <c r="N213" t="n">
         <v>0</v>
       </c>
+      <c r="O213" t="n">
+        <v>3.6</v>
+      </c>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
@@ -10728,6 +11369,9 @@
       <c r="N214" t="n">
         <v>0</v>
       </c>
+      <c r="O214" t="n">
+        <v>2.6</v>
+      </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
@@ -10776,6 +11420,9 @@
       <c r="N215" t="n">
         <v>0</v>
       </c>
+      <c r="O215" t="n">
+        <v>5.6</v>
+      </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
@@ -10822,7 +11469,10 @@
         </is>
       </c>
       <c r="N216" t="n">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="O216" t="n">
+        <v>22.8</v>
       </c>
     </row>
     <row r="217">
@@ -10872,6 +11522,9 @@
       <c r="N217" t="n">
         <v>0</v>
       </c>
+      <c r="O217" t="n">
+        <v>22.6</v>
+      </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
@@ -10920,6 +11573,9 @@
       <c r="N218" t="n">
         <v>0</v>
       </c>
+      <c r="O218" t="n">
+        <v>24.5</v>
+      </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
@@ -10968,6 +11624,9 @@
       <c r="N219" t="n">
         <v>0</v>
       </c>
+      <c r="O219" t="n">
+        <v>0.9</v>
+      </c>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
@@ -11016,6 +11675,9 @@
       <c r="N220" t="n">
         <v>0</v>
       </c>
+      <c r="O220" t="n">
+        <v>8.5</v>
+      </c>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
@@ -11064,6 +11726,9 @@
       <c r="N221" t="n">
         <v>0</v>
       </c>
+      <c r="O221" t="n">
+        <v>11.8</v>
+      </c>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
@@ -11112,6 +11777,9 @@
       <c r="N222" t="n">
         <v>0</v>
       </c>
+      <c r="O222" t="n">
+        <v>19.1</v>
+      </c>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
@@ -11160,6 +11828,9 @@
       <c r="N223" t="n">
         <v>0</v>
       </c>
+      <c r="O223" t="n">
+        <v>3.6</v>
+      </c>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
@@ -11208,6 +11879,9 @@
       <c r="N224" t="n">
         <v>0</v>
       </c>
+      <c r="O224" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
@@ -11256,6 +11930,9 @@
       <c r="N225" t="n">
         <v>0</v>
       </c>
+      <c r="O225" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
@@ -11304,6 +11981,9 @@
       <c r="N226" t="n">
         <v>0</v>
       </c>
+      <c r="O226" t="n">
+        <v>2.3</v>
+      </c>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
@@ -11352,6 +12032,9 @@
       <c r="N227" t="n">
         <v>0</v>
       </c>
+      <c r="O227" t="n">
+        <v>14</v>
+      </c>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
@@ -11400,6 +12083,9 @@
       <c r="N228" t="n">
         <v>0</v>
       </c>
+      <c r="O228" t="n">
+        <v>14.5</v>
+      </c>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
@@ -11448,6 +12134,9 @@
       <c r="N229" t="n">
         <v>0</v>
       </c>
+      <c r="O229" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
@@ -11496,6 +12185,9 @@
       <c r="N230" t="n">
         <v>0</v>
       </c>
+      <c r="O230" t="n">
+        <v>24</v>
+      </c>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
@@ -11544,6 +12236,9 @@
       <c r="N231" t="n">
         <v>0</v>
       </c>
+      <c r="O231" t="n">
+        <v>12.7</v>
+      </c>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
@@ -11592,6 +12287,9 @@
       <c r="N232" t="n">
         <v>0</v>
       </c>
+      <c r="O232" t="n">
+        <v>10.9</v>
+      </c>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
@@ -11640,6 +12338,9 @@
       <c r="N233" t="n">
         <v>0</v>
       </c>
+      <c r="O233" t="n">
+        <v>10.9</v>
+      </c>
     </row>
     <row r="234">
       <c r="A234" t="inlineStr">
@@ -11688,6 +12389,9 @@
       <c r="N234" t="n">
         <v>0</v>
       </c>
+      <c r="O234" t="n">
+        <v>15.8</v>
+      </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
@@ -11736,6 +12440,9 @@
       <c r="N235" t="n">
         <v>0</v>
       </c>
+      <c r="O235" t="n">
+        <v>4.5</v>
+      </c>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
@@ -11784,6 +12491,9 @@
       <c r="N236" t="n">
         <v>0</v>
       </c>
+      <c r="O236" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
@@ -11832,6 +12542,9 @@
       <c r="N237" t="n">
         <v>0</v>
       </c>
+      <c r="O237" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
@@ -11880,6 +12593,9 @@
       <c r="N238" t="n">
         <v>0</v>
       </c>
+      <c r="O238" t="n">
+        <v>11.9</v>
+      </c>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
@@ -11928,6 +12644,9 @@
       <c r="N239" t="n">
         <v>0</v>
       </c>
+      <c r="O239" t="n">
+        <v>24</v>
+      </c>
     </row>
     <row r="240">
       <c r="A240" t="inlineStr">
@@ -11976,6 +12695,9 @@
       <c r="N240" t="n">
         <v>0</v>
       </c>
+      <c r="O240" t="n">
+        <v>16.3</v>
+      </c>
     </row>
     <row r="241">
       <c r="A241" t="inlineStr">
@@ -12024,6 +12746,9 @@
       <c r="N241" t="n">
         <v>0</v>
       </c>
+      <c r="O241" t="n">
+        <v>15.5</v>
+      </c>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
@@ -12072,6 +12797,9 @@
       <c r="N242" t="n">
         <v>0</v>
       </c>
+      <c r="O242" t="n">
+        <v>4.5</v>
+      </c>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
@@ -12120,6 +12848,9 @@
       <c r="N243" t="n">
         <v>0</v>
       </c>
+      <c r="O243" t="n">
+        <v>27.7</v>
+      </c>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
@@ -12168,6 +12899,9 @@
       <c r="N244" t="n">
         <v>0</v>
       </c>
+      <c r="O244" t="n">
+        <v>8.9</v>
+      </c>
     </row>
     <row r="245">
       <c r="A245" t="inlineStr">
@@ -12216,6 +12950,9 @@
       <c r="N245" t="n">
         <v>0</v>
       </c>
+      <c r="O245" t="n">
+        <v>8.9</v>
+      </c>
     </row>
     <row r="246">
       <c r="A246" t="inlineStr">
@@ -12262,7 +12999,10 @@
         </is>
       </c>
       <c r="N246" t="n">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="O246" t="n">
+        <v>23</v>
       </c>
     </row>
     <row r="247">
@@ -12312,6 +13052,9 @@
       <c r="N247" t="n">
         <v>0</v>
       </c>
+      <c r="O247" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
@@ -12360,6 +13103,9 @@
       <c r="N248" t="n">
         <v>0</v>
       </c>
+      <c r="O248" t="n">
+        <v>8.800000000000001</v>
+      </c>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
@@ -12406,7 +13152,10 @@
         </is>
       </c>
       <c r="N249" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="O249" t="n">
+        <v>7.8</v>
       </c>
     </row>
     <row r="250">
@@ -12456,6 +13205,9 @@
       <c r="N250" t="n">
         <v>0</v>
       </c>
+      <c r="O250" t="n">
+        <v>26</v>
+      </c>
     </row>
     <row r="251">
       <c r="A251" t="inlineStr">
@@ -12504,6 +13256,9 @@
       <c r="N251" t="n">
         <v>0</v>
       </c>
+      <c r="O251" t="n">
+        <v>9.1</v>
+      </c>
     </row>
     <row r="252">
       <c r="A252" t="inlineStr">
@@ -12552,6 +13307,9 @@
       <c r="N252" t="n">
         <v>0</v>
       </c>
+      <c r="O252" t="n">
+        <v>24.8</v>
+      </c>
     </row>
     <row r="253">
       <c r="A253" t="inlineStr">
@@ -12598,7 +13356,10 @@
         </is>
       </c>
       <c r="N253" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="O253" t="n">
+        <v>2.4</v>
       </c>
     </row>
     <row r="254">
@@ -12648,6 +13409,9 @@
       <c r="N254" t="n">
         <v>0</v>
       </c>
+      <c r="O254" t="n">
+        <v>11.6</v>
+      </c>
     </row>
     <row r="255">
       <c r="A255" t="inlineStr">
@@ -12696,6 +13460,9 @@
       <c r="N255" t="n">
         <v>0</v>
       </c>
+      <c r="O255" t="n">
+        <v>6.7</v>
+      </c>
     </row>
     <row r="256">
       <c r="A256" t="inlineStr">
@@ -12744,6 +13511,9 @@
       <c r="N256" t="n">
         <v>0</v>
       </c>
+      <c r="O256" t="n">
+        <v>7.4</v>
+      </c>
     </row>
     <row r="257">
       <c r="A257" t="inlineStr">
@@ -12792,6 +13562,9 @@
       <c r="N257" t="n">
         <v>0</v>
       </c>
+      <c r="O257" t="n">
+        <v>7.3</v>
+      </c>
     </row>
     <row r="258">
       <c r="A258" t="inlineStr">
@@ -12840,6 +13613,9 @@
       <c r="N258" t="n">
         <v>0</v>
       </c>
+      <c r="O258" t="n">
+        <v>27</v>
+      </c>
     </row>
     <row r="259">
       <c r="A259" t="inlineStr">
@@ -12888,6 +13664,9 @@
       <c r="N259" t="n">
         <v>0</v>
       </c>
+      <c r="O259" t="n">
+        <v>19.5</v>
+      </c>
     </row>
     <row r="260">
       <c r="A260" t="inlineStr">
@@ -12936,6 +13715,9 @@
       <c r="N260" t="n">
         <v>0</v>
       </c>
+      <c r="O260" t="n">
+        <v>11.3</v>
+      </c>
     </row>
     <row r="261">
       <c r="A261" t="inlineStr">
@@ -12984,6 +13766,9 @@
       <c r="N261" t="n">
         <v>0</v>
       </c>
+      <c r="O261" t="n">
+        <v>21.9</v>
+      </c>
     </row>
     <row r="262">
       <c r="A262" t="inlineStr">
@@ -13032,6 +13817,9 @@
       <c r="N262" t="n">
         <v>0</v>
       </c>
+      <c r="O262" t="n">
+        <v>15.6</v>
+      </c>
     </row>
     <row r="263">
       <c r="A263" t="inlineStr">
@@ -13080,6 +13868,9 @@
       <c r="N263" t="n">
         <v>0</v>
       </c>
+      <c r="O263" t="n">
+        <v>7.7</v>
+      </c>
     </row>
     <row r="264">
       <c r="A264" t="inlineStr">
@@ -13128,6 +13919,9 @@
       <c r="N264" t="n">
         <v>0</v>
       </c>
+      <c r="O264" t="n">
+        <v>12.1</v>
+      </c>
     </row>
     <row r="265">
       <c r="A265" t="inlineStr">
@@ -13176,6 +13970,9 @@
       <c r="N265" t="n">
         <v>0</v>
       </c>
+      <c r="O265" t="n">
+        <v>10.4</v>
+      </c>
     </row>
     <row r="266">
       <c r="A266" t="inlineStr">
@@ -13224,6 +14021,9 @@
       <c r="N266" t="n">
         <v>0</v>
       </c>
+      <c r="O266" t="n">
+        <v>5.8</v>
+      </c>
     </row>
     <row r="267">
       <c r="A267" t="inlineStr">
@@ -13272,6 +14072,9 @@
       <c r="N267" t="n">
         <v>0</v>
       </c>
+      <c r="O267" t="n">
+        <v>7.8</v>
+      </c>
     </row>
     <row r="268">
       <c r="A268" t="inlineStr">
@@ -13320,6 +14123,9 @@
       <c r="N268" t="n">
         <v>0</v>
       </c>
+      <c r="O268" t="n">
+        <v>7.5</v>
+      </c>
     </row>
     <row r="269">
       <c r="A269" t="inlineStr">
@@ -13368,6 +14174,9 @@
       <c r="N269" t="n">
         <v>0</v>
       </c>
+      <c r="O269" t="n">
+        <v>7.1</v>
+      </c>
     </row>
     <row r="270">
       <c r="A270" t="inlineStr">
@@ -13416,6 +14225,9 @@
       <c r="N270" t="n">
         <v>0</v>
       </c>
+      <c r="O270" t="n">
+        <v>7.6</v>
+      </c>
     </row>
     <row r="271">
       <c r="A271" t="inlineStr">
@@ -13462,7 +14274,10 @@
         </is>
       </c>
       <c r="N271" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="O271" t="n">
+        <v>3.2</v>
       </c>
     </row>
     <row r="272">
@@ -13512,6 +14327,9 @@
       <c r="N272" t="n">
         <v>0</v>
       </c>
+      <c r="O272" t="n">
+        <v>2.5</v>
+      </c>
     </row>
     <row r="273">
       <c r="A273" t="inlineStr">
@@ -13560,6 +14378,9 @@
       <c r="N273" t="n">
         <v>0</v>
       </c>
+      <c r="O273" t="n">
+        <v>15.2</v>
+      </c>
     </row>
     <row r="274">
       <c r="A274" t="inlineStr">
@@ -13608,6 +14429,9 @@
       <c r="N274" t="n">
         <v>0</v>
       </c>
+      <c r="O274" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="275">
       <c r="A275" t="inlineStr">
@@ -13656,6 +14480,9 @@
       <c r="N275" t="n">
         <v>0</v>
       </c>
+      <c r="O275" t="n">
+        <v>17</v>
+      </c>
     </row>
     <row r="276">
       <c r="A276" t="inlineStr">
@@ -13704,6 +14531,9 @@
       <c r="N276" t="n">
         <v>0</v>
       </c>
+      <c r="O276" t="n">
+        <v>12.4</v>
+      </c>
     </row>
     <row r="277">
       <c r="A277" t="inlineStr">
@@ -13752,6 +14582,9 @@
       <c r="N277" t="n">
         <v>0</v>
       </c>
+      <c r="O277" t="n">
+        <v>18.5</v>
+      </c>
     </row>
     <row r="278">
       <c r="A278" t="inlineStr">
@@ -13800,6 +14633,9 @@
       <c r="N278" t="n">
         <v>0</v>
       </c>
+      <c r="O278" t="n">
+        <v>18.4</v>
+      </c>
     </row>
     <row r="279">
       <c r="A279" t="inlineStr">
@@ -13848,6 +14684,9 @@
       <c r="N279" t="n">
         <v>0</v>
       </c>
+      <c r="O279" t="n">
+        <v>21.3</v>
+      </c>
     </row>
     <row r="280">
       <c r="A280" t="inlineStr">
@@ -13896,6 +14735,9 @@
       <c r="N280" t="n">
         <v>0</v>
       </c>
+      <c r="O280" t="n">
+        <v>21.9</v>
+      </c>
     </row>
     <row r="281">
       <c r="A281" t="inlineStr">
@@ -13944,6 +14786,9 @@
       <c r="N281" t="n">
         <v>0</v>
       </c>
+      <c r="O281" t="n">
+        <v>5.7</v>
+      </c>
     </row>
     <row r="282">
       <c r="A282" t="inlineStr">
@@ -13992,6 +14837,9 @@
       <c r="N282" t="n">
         <v>0</v>
       </c>
+      <c r="O282" t="n">
+        <v>18.5</v>
+      </c>
     </row>
     <row r="283">
       <c r="A283" t="inlineStr">
@@ -14040,6 +14888,9 @@
       <c r="N283" t="n">
         <v>0</v>
       </c>
+      <c r="O283" t="n">
+        <v>17.4</v>
+      </c>
     </row>
     <row r="284">
       <c r="A284" t="inlineStr">
@@ -14088,6 +14939,9 @@
       <c r="N284" t="n">
         <v>0</v>
       </c>
+      <c r="O284" t="n">
+        <v>30.3</v>
+      </c>
     </row>
     <row r="285">
       <c r="A285" t="inlineStr">
@@ -14136,6 +14990,9 @@
       <c r="N285" t="n">
         <v>0</v>
       </c>
+      <c r="O285" t="n">
+        <v>6.4</v>
+      </c>
     </row>
     <row r="286">
       <c r="A286" t="inlineStr">
@@ -14184,6 +15041,9 @@
       <c r="N286" t="n">
         <v>0</v>
       </c>
+      <c r="O286" t="n">
+        <v>13.9</v>
+      </c>
     </row>
     <row r="287">
       <c r="A287" t="inlineStr">
@@ -14232,6 +15092,9 @@
       <c r="N287" t="n">
         <v>0</v>
       </c>
+      <c r="O287" t="n">
+        <v>2.7</v>
+      </c>
     </row>
     <row r="288">
       <c r="A288" t="inlineStr">
@@ -14280,6 +15143,9 @@
       <c r="N288" t="n">
         <v>0</v>
       </c>
+      <c r="O288" t="n">
+        <v>1.7</v>
+      </c>
     </row>
     <row r="289">
       <c r="A289" t="inlineStr">
@@ -14328,6 +15194,9 @@
       <c r="N289" t="n">
         <v>0</v>
       </c>
+      <c r="O289" t="n">
+        <v>15.8</v>
+      </c>
     </row>
     <row r="290">
       <c r="A290" t="inlineStr">
@@ -14376,6 +15245,9 @@
       <c r="N290" t="n">
         <v>0</v>
       </c>
+      <c r="O290" t="n">
+        <v>64.3</v>
+      </c>
     </row>
     <row r="291">
       <c r="A291" t="inlineStr">
@@ -14424,6 +15296,9 @@
       <c r="N291" t="n">
         <v>0</v>
       </c>
+      <c r="O291" t="n">
+        <v>22</v>
+      </c>
     </row>
     <row r="292">
       <c r="A292" t="inlineStr">
@@ -14472,6 +15347,9 @@
       <c r="N292" t="n">
         <v>0</v>
       </c>
+      <c r="O292" t="n">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="293">
       <c r="A293" t="inlineStr">
@@ -14520,6 +15398,9 @@
       <c r="N293" t="n">
         <v>0</v>
       </c>
+      <c r="O293" t="n">
+        <v>30.8</v>
+      </c>
     </row>
     <row r="294">
       <c r="A294" t="inlineStr">
@@ -14568,6 +15449,9 @@
       <c r="N294" t="n">
         <v>0</v>
       </c>
+      <c r="O294" t="n">
+        <v>9.5</v>
+      </c>
     </row>
     <row r="295">
       <c r="A295" t="inlineStr">
@@ -14615,6 +15499,9 @@
       </c>
       <c r="N295" t="n">
         <v>0</v>
+      </c>
+      <c r="O295" t="n">
+        <v>18.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>